<commit_message>
Realizado extração dos dados com sucesso
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Rua Pedro Doll, 564</t>
         </is>
       </c>
     </row>
@@ -520,17 +520,17 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>151</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Rua Francisca Júlia, 524</t>
         </is>
       </c>
     </row>
@@ -547,24 +547,24 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>118</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Conselheiro Saraiva, 207</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>BlueFit Santana</t>
+          <t>Black Fitness Club</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -574,24 +574,24 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>196</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Gaspar Soares, 88</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Black Fitness Club</t>
+          <t>BlueFit Santana</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -601,24 +601,24 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>691</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Dr. Zuquim, 1872</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Tracer Parkour - Santana</t>
+          <t>Health Academy</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -628,24 +628,24 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Voluntários da Pátria, 2468 - Conjunto 167</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Health Academy</t>
+          <t>Tracer Parkour - Santana</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -655,24 +655,24 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Dr. Zuquim, 859</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Academia Butterfly</t>
+          <t>Silver | Fitness &amp; Spa | Santana - Zona Norte - SP</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -682,24 +682,24 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Conselheiro Moreira de Barros, 636</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Silver | Fitness &amp; Spa | Santana - Zona Norte - SP</t>
+          <t>Academia Butterfly</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -709,17 +709,17 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>148</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Conselheiro Moreira de Barros, 221</t>
         </is>
       </c>
     </row>
@@ -736,17 +736,17 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>3,9</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>156</t>
         </is>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Rua Dr. Olavo Egídio, 632</t>
         </is>
       </c>
     </row>
@@ -763,17 +763,17 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>18</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Rua Benvinda Aparecida de Abreu Leme, 43 - Sala 3</t>
         </is>
       </c>
     </row>
@@ -790,17 +790,17 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>233</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Ten. Blum, 93</t>
         </is>
       </c>
     </row>
@@ -817,17 +817,17 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>151</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Francisca Júlia, 524</t>
         </is>
       </c>
     </row>
@@ -844,17 +844,17 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>510</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Rua Chemin Del Pra, 58</t>
         </is>
       </c>
     </row>
@@ -871,17 +871,17 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Conselheiro Moreira de Barros, 711</t>
         </is>
       </c>
     </row>
@@ -898,17 +898,17 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Av. Nova Cantareira, 624</t>
         </is>
       </c>
     </row>
@@ -925,17 +925,17 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,1</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>598</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>Av. Luiz Dumont Villares, 200</t>
         </is>
       </c>
     </row>
@@ -952,17 +952,17 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>1.293</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Mateus Leme, 114</t>
         </is>
       </c>
     </row>
@@ -984,12 +984,12 @@
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>254</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Voluntários da Pátria, 1884</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>Academia · 564 Rua Pedro Doll</t>
+          <t>R. Pedro Doll, 564</t>
         </is>
       </c>
     </row>
@@ -1043,14 +1043,14 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Antônio Pereira de Sousa, 227</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Lassù</t>
+          <t>Angusteria</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -1060,24 +1060,24 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>443</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Duarte de Azevedo, 468</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Famiglia Mancini Trattoria</t>
+          <t>Lassù</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
@@ -1087,24 +1087,24 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>3.332</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Conselheiro Saraiva, 207</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>La Mordida</t>
+          <t>Famiglia Mancini Trattoria</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -1114,24 +1114,24 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>27.903</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>Rua Avanhandava, 81, Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Rainha da Jovita</t>
+          <t>La Mordida</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
@@ -1141,24 +1141,24 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>618</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Prof. Lourival Gomes Machado, 274 - 272</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>La Ficazza</t>
+          <t>Rainha da Jovita</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
@@ -1168,24 +1168,24 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>172</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>Rua Dr. Olavo Egídio, 449</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>Sabor de Santana</t>
+          <t>La Ficazza</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
@@ -1195,24 +1195,24 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>730</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Dr. César, 1160</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>LeLui Bar e Cozinha</t>
+          <t>Sabor de Santana</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -1222,24 +1222,24 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>194</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Duarte de Azevedo, 352</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>Dom ramiro</t>
+          <t>LeLui Bar e Cozinha</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
@@ -1249,24 +1249,24 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>1.018</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Jacuna, 302</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>Angusteria</t>
+          <t>Dom ramiro</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -1276,17 +1276,17 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>3.579</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Dr. César, 105</t>
         </is>
       </c>
     </row>
@@ -1303,24 +1303,24 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>114</t>
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Dr. Zuquim, 1941</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>Santo Mar Restaurante — Unidade Santana</t>
+          <t>Salvi Café e Cozinha - Santana</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
@@ -1330,24 +1330,24 @@
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>1.216</t>
         </is>
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Tupiguaes, 140</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Salvi Café e Cozinha - Santana</t>
+          <t>Pecorino Cucina Mediterranea Braz Leme: Restaurante, Delivery São Paulo SP</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -1357,24 +1357,24 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>1.549</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>Av. Braz Leme, 1200</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>Pecorino Cucina Mediterranea Braz Leme: Restaurante, Delivery São Paulo SP</t>
+          <t>Santo Mar Restaurante — Unidade Santana</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
@@ -1389,12 +1389,12 @@
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>3.898</t>
         </is>
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>Av. Luiz Dumont Villares, 1306</t>
         </is>
       </c>
     </row>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,2</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>363</t>
         </is>
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Prof. Lourival Gomes Machado, 273</t>
         </is>
       </c>
     </row>
@@ -1443,19 +1443,19 @@
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>1.741</t>
         </is>
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Lucas de Freitas de Azevedo, 87</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>La Braciera Pizzaria - Pizza Napoletana</t>
+          <t>Quintal Brasil</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -1465,24 +1465,24 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,2</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>770</t>
         </is>
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Alfredo Pujol, 853</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>Quintal Brasil</t>
+          <t>La Braciera Pizzaria - Pizza Napoletana</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -1492,17 +1492,17 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>4.166</t>
         </is>
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Conselheiro Saraiva, 664</t>
         </is>
       </c>
     </row>
@@ -1519,17 +1519,17 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>572</t>
         </is>
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Voluntários da Pátria, 3670</t>
         </is>
       </c>
     </row>
@@ -1546,17 +1546,17 @@
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>45.025</t>
         </is>
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Portuguesa ·  · R. Antônio Pereira de Sousa, 227</t>
+          <t>Av. Braz Leme, 201</t>
         </is>
       </c>
     </row>
@@ -1583,14 +1583,14 @@
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Augusto Tolle, 279</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>Latte di Fiori</t>
+          <t>Paleteria paulista - unidade Santana</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
@@ -1605,19 +1605,19 @@
       </c>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Rua Dr. Olavo Egídio, 798</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>Paleteria paulista - unidade Santana</t>
+          <t>Latte di Fiori</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -1632,12 +1632,12 @@
       </c>
       <c r="D44" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>416</t>
         </is>
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Águas de São Pedro, 427</t>
         </is>
       </c>
     </row>
@@ -1654,17 +1654,17 @@
       </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>69</t>
         </is>
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Nova Cantareira, 346</t>
         </is>
       </c>
     </row>
@@ -1681,24 +1681,24 @@
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>304</t>
         </is>
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Dom Henrique Mourão, 216</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>Candy Village Sorvete Infancia vintage</t>
+          <t>Gelato Borelli Santana</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -1708,24 +1708,24 @@
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>431</t>
         </is>
       </c>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Tupiguaes, 48 - Loja 02</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>Gelato Borelli Santana</t>
+          <t>Bacio di Latte - Augusto Tolle</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -1735,24 +1735,24 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>143</t>
         </is>
       </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Augusto Tolle, 619</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>Bacio di Latte - Augusto Tolle</t>
+          <t>Lambisk Sorvetes</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -1762,24 +1762,24 @@
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>192</t>
         </is>
       </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Rua Conselheiro Moreira de Barros, 1002</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>Lambisk Sorvetes</t>
+          <t>Frida &amp; Mina Sorveteria</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -1789,24 +1789,24 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>6.987</t>
         </is>
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Artur de Azevedo, 1147</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>Frida &amp; Mina Sorveteria</t>
+          <t>OGGI SORVETES PARADA INGLESA</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -1816,24 +1816,24 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>378</t>
         </is>
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Gen. Ataliba Leonel, 1976</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>OGGI SORVETES PARADA INGLESA</t>
+          <t>Dezato Gelato - Braz Leme</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -1848,19 +1848,19 @@
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>260</t>
         </is>
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Braz Leme, 1200 - Loja 06</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>Dezato Gelato - Braz Leme</t>
+          <t>Sorveteria do Centro</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -1870,17 +1870,17 @@
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>2.875</t>
         </is>
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Epitácio Pessoa, 94</t>
         </is>
       </c>
     </row>
@@ -1897,24 +1897,24 @@
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>31</t>
         </is>
       </c>
       <c r="E54" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Nova Cantareira, 335</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>Sorveteria Lafer &amp; Açaí</t>
+          <t>Candy Village Sorvete Infancia vintage</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -1924,24 +1924,24 @@
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Jovita</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>Sou Ice Santa Teresinha - Sorvetes e Congelados</t>
+          <t>Sorveteria Lafer &amp; Açaí</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -1951,24 +1951,24 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>982</t>
         </is>
       </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Maria Curupaiti, 1520</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>Sorveteria do Centro</t>
+          <t>Sou Ice Santa Teresinha - Sorvetes e Congelados</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -1983,12 +1983,12 @@
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>49</t>
         </is>
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>R. Conselheiro Moreira de Barros, 1309 - Loja 01</t>
         </is>
       </c>
     </row>
@@ -2005,17 +2005,17 @@
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>1.593</t>
         </is>
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Braz Leme, 2378</t>
         </is>
       </c>
     </row>
@@ -2032,17 +2032,17 @@
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>135</t>
         </is>
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Conceição, 898</t>
         </is>
       </c>
     </row>
@@ -2059,24 +2059,24 @@
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>87</t>
         </is>
       </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Av. Gen. Ataliba Leonel, 3837</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>Tutti Crema Gelato</t>
+          <t>Bacio di Latte</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -2086,17 +2086,17 @@
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>504</t>
+          <t>807</t>
         </is>
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>Sorvete ·  · R. Augusto Tolle, 279</t>
+          <t>Tv. Casalbuono, 120</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajuste no Readme/ E na padronização dos dados coletados das ruas
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -450,7 +450,7 @@
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="53" customWidth="1" min="5" max="5"/>
+    <col width="52" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,7 +483,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>BIO RITMO Academia | Pedro Doll</t>
+          <t>Academia Motion Fit - Limoeiro</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -493,24 +493,24 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>3,9</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>154</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Rua Pedro Doll, 564</t>
+          <t>Av. Augusto Antunes, 546</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>30'fit - Treinamento Funcional</t>
+          <t>BIO RITMO Academia | Pedro Doll</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -520,17 +520,17 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>5,0</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>319</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Rua Francisca Júlia, 524</t>
+          <t>R. Pedro Doll, 564</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Tracer Parkour - Santana</t>
+          <t>Silver | Fitness &amp; Spa | Santana - Zona Norte - SP</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -660,19 +660,19 @@
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>R. Dr. Zuquim, 859</t>
+          <t>R. Conselheiro Moreira de Barros, 636</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Silver | Fitness &amp; Spa | Santana - Zona Norte - SP</t>
+          <t>Academia Butterfly</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -682,24 +682,24 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>148</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Moreira de Barros, 636</t>
+          <t>R. Conselheiro Moreira de Barros, 221</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Academia Butterfly</t>
+          <t>Tracer Parkour - Santana</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -709,17 +709,17 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>52</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Moreira de Barros, 221</t>
+          <t>R. Dr. Zuquim, 859</t>
         </is>
       </c>
     </row>
@@ -746,14 +746,14 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>Rua Dr. Olavo Egídio, 632</t>
+          <t>R. Dr. Olavo Egídio, 632</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Studio JD Treinos Coletivos</t>
+          <t>Academia Acqua Ville</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -763,24 +763,24 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>233</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Rua Benvinda Aparecida de Abreu Leme, 43 - Sala 3</t>
+          <t>R. Ten. Blum, 93</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Academia Acqua Ville</t>
+          <t>30'fit - Treinamento Funcional</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -790,24 +790,24 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>233</t>
+          <t>152</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>R. Ten. Blum, 93</t>
+          <t>R. Francisca Júlia, 524</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>30'fit - Treinamento Funcional</t>
+          <t>High Point Academia</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -817,24 +817,24 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>5,0</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>510</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>R. Francisca Júlia, 524</t>
+          <t>R. Chemin Del Pra, 58</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>High Point Academia</t>
+          <t>Studio Livinng</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -844,24 +844,24 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>510</t>
+          <t>166</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Rua Chemin Del Pra, 58</t>
+          <t>R. Conselheiro Moreira de Barros, 711</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Studio Livinng</t>
+          <t>PERSONAL S/A - Academia de Treinamento Funcional no Jardim São Paulo</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -871,24 +871,24 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Moreira de Barros, 711</t>
+          <t>Av. Nova Cantareira, 624</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>PERSONAL S/A - Academia de Treinamento Funcional no Jardim São Paulo</t>
+          <t>Academia K2 Fitness Technology</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -898,24 +898,24 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,1</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>598</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Av. Nova Cantareira, 624</t>
+          <t>Av. Luiz Dumont Villares, 200</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>Academia K2 Fitness Technology</t>
+          <t>BW Academia | Santana - Zona Norte - São Paulo</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
@@ -925,24 +925,24 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>4,1</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>598</t>
+          <t>1.293</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Av. Luiz Dumont Villares, 200</t>
+          <t>R. Mateus Leme, 114</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>BW Academia | Santana - Zona Norte - São Paulo</t>
+          <t>Smarkim Gym Academia</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -952,24 +952,24 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>254</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>R. Mateus Leme, 114</t>
+          <t>R. Voluntários da Pátria, 1884</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Smarkim Gym Academia</t>
+          <t>Studio JD Treinos Coletivos</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
@@ -979,17 +979,17 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>R. Voluntários da Pátria, 1884</t>
+          <t>R. Benvinda Aparecida de Abreu Leme, 43 - Sala 3</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Restaurante Dona Florinda</t>
+          <t>Lassù</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -1033,24 +1033,24 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>3.332</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>R. Antônio Pereira de Sousa, 227</t>
+          <t>R. Conselheiro Saraiva, 207</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Angusteria</t>
+          <t>Restaurante Dona Florinda</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -1060,24 +1060,24 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>443</t>
+          <t>1.012</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>R. Duarte de Azevedo, 468</t>
+          <t>R. Antônio Pereira de Sousa, 227</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Lassù</t>
+          <t>Angusteria</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
@@ -1087,24 +1087,24 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>3.332</t>
+          <t>443</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Saraiva, 207</t>
+          <t>R. Duarte de Azevedo, 468</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>Famiglia Mancini Trattoria</t>
+          <t>La Braciera Pizzaria - Pizza Napoletana</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -1114,24 +1114,24 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>27.903</t>
+          <t>4.166</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Rua Avanhandava, 81, Bela Vista</t>
+          <t>R. Conselheiro Saraiva, 664</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>La Mordida</t>
+          <t>La Crosta Forneria</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
@@ -1141,24 +1141,24 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>1.464</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>R. Prof. Lourival Gomes Machado, 274 - 272</t>
+          <t>R. Pontins, 52</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>Rainha da Jovita</t>
+          <t>Famiglia Mancini Trattoria</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
@@ -1168,24 +1168,24 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>27.906</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Rua Dr. Olavo Egídio, 449</t>
+          <t>R. Avanhandava, 81, Bela Vista</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>La Ficazza</t>
+          <t>Sargento Garcia</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
@@ -1195,24 +1195,24 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>730</t>
+          <t>886</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>R. Dr. César, 1160</t>
+          <t>R. Padre Luciano, 154</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>Sabor de Santana</t>
+          <t>Rainha da Jovita</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -1227,19 +1227,19 @@
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>172</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>R. Duarte de Azevedo, 352</t>
+          <t>R. Dr. Olavo Egídio, 449</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>LeLui Bar e Cozinha</t>
+          <t>La Ficazza</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
@@ -1249,24 +1249,24 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>1.018</t>
+          <t>730</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>R. Jacuna, 302</t>
+          <t>R. Dr. César, 1160</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>Dom ramiro</t>
+          <t>Seu Manuel Restaurante</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -1276,24 +1276,24 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>3.579</t>
+          <t>519</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>R. Dr. César, 105</t>
+          <t>R. Ismael Neri, 441</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>Restaurante Nova Zuquim (Alto de Santana)</t>
+          <t>Sabor de Santana</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
@@ -1303,24 +1303,24 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>194</t>
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>R. Dr. Zuquim, 1941</t>
+          <t>R. Duarte de Azevedo, 352</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>Salvi Café e Cozinha - Santana</t>
+          <t>Dona Carmela</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
@@ -1330,24 +1330,24 @@
       </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>3.595</t>
         </is>
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>R. Tupiguaes, 140</t>
+          <t>R. Dr. César, 944</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>Pecorino Cucina Mediterranea Braz Leme: Restaurante, Delivery São Paulo SP</t>
+          <t>Crostini Osteria</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -1357,24 +1357,24 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>410</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Av. Braz Leme, 1200</t>
+          <t>R. Dr. César, 1243</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>Santo Mar Restaurante — Unidade Santana</t>
+          <t>Restaurante Nova Zuquim (Alto de Santana)</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
@@ -1384,24 +1384,24 @@
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>3.898</t>
+          <t>114</t>
         </is>
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Av. Luiz Dumont Villares, 1306</t>
+          <t>R. Dr. Zuquim, 1941</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>Una Rooftop Restaurante &amp; Bar</t>
+          <t>Salvi Café e Cozinha - Santana</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
@@ -1411,24 +1411,24 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>4,2</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>363</t>
+          <t>1.216</t>
         </is>
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>R. Prof. Lourival Gomes Machado, 273</t>
+          <t>R. Tupiguaes, 140</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>Restaurante Fulô - Cozinha Regional</t>
+          <t>LeLui Bar e Cozinha</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -1438,24 +1438,24 @@
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>1.741</t>
+          <t>1.018</t>
         </is>
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>R. Lucas de Freitas de Azevedo, 87</t>
+          <t>R. Jacuna, 302</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>Quintal Brasil</t>
+          <t>Aoka Parrilla e Bar</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -1465,24 +1465,24 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>4,2</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>770</t>
+          <t>238</t>
         </is>
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>R. Alfredo Pujol, 853</t>
+          <t>Av. Leôncio de Magalhães, 84</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>La Braciera Pizzaria - Pizza Napoletana</t>
+          <t>Santo Mar Restaurante — Unidade Santana</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -1492,24 +1492,24 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>4.166</t>
+          <t>3.898</t>
         </is>
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Saraiva, 664</t>
+          <t>Av. Luiz Dumont Villares, 1306</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>Point Santana</t>
+          <t>Dom ramiro</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -1519,24 +1519,24 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t>572</t>
+          <t>3.579</t>
         </is>
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>R. Voluntários da Pátria, 3670</t>
+          <t>R. Dr. César, 105</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>Restaurante Coco Bambu Anhembi</t>
+          <t>Pecorino Cucina Mediterranea Braz Leme: Restaurante, Delivery São Paulo SP</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -1546,17 +1546,17 @@
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
         <is>
-          <t>45.025</t>
+          <t>1.549</t>
         </is>
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Av. Braz Leme, 201</t>
+          <t>Av. Braz Leme, 1200</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>Paleteria paulista - unidade Santana</t>
+          <t>Latte di Fiori</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
@@ -1605,19 +1605,19 @@
       </c>
       <c r="D43" s="2" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>416</t>
         </is>
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>Rua Dr. Olavo Egídio, 798</t>
+          <t>Av. Águas de São Pedro, 427</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>Latte di Fiori</t>
+          <t>Paleteria paulista - unidade Santana</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -1632,19 +1632,19 @@
       </c>
       <c r="D44" s="2" t="inlineStr">
         <is>
-          <t>416</t>
+          <t>99</t>
         </is>
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>Av. Águas de São Pedro, 427</t>
+          <t>R. Dr. Olavo Egídio, 798</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>Sou ice - Sorvetes e Congelados</t>
+          <t>Sorvetes Rochinha Santana</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -1659,19 +1659,19 @@
       </c>
       <c r="D45" s="2" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>304</t>
         </is>
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>Av. Nova Cantareira, 346</t>
+          <t>R. Dom Henrique Mourão, 216</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>Sorvetes Rochinha Santana</t>
+          <t>Gelato Borelli Santana</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -1681,24 +1681,24 @@
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
         <is>
-          <t>304</t>
+          <t>431</t>
         </is>
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>R. Dom Henrique Mourão, 216</t>
+          <t>R. Tupiguaes, 48 - Loja 02</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>Gelato Borelli Santana</t>
+          <t>Bacio di Latte - Augusto Tolle</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -1708,24 +1708,24 @@
       </c>
       <c r="C47" s="2" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D47" s="2" t="inlineStr">
         <is>
-          <t>431</t>
+          <t>143</t>
         </is>
       </c>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>R. Tupiguaes, 48 - Loja 02</t>
+          <t>R. Augusto Tolle, 619</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>Bacio di Latte - Augusto Tolle</t>
+          <t>Frida &amp; Mina Sorveteria</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -1735,24 +1735,24 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>6.987</t>
         </is>
       </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>R. Augusto Tolle, 619</t>
+          <t>R. Artur de Azevedo, 1147</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>Lambisk Sorvetes</t>
+          <t>Dezato Gelato - Braz Leme</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -1762,24 +1762,24 @@
       </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D49" s="2" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>260</t>
         </is>
       </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>Rua Conselheiro Moreira de Barros, 1002</t>
+          <t>Av. Braz Leme, 1200 - Loja 06</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>Frida &amp; Mina Sorveteria</t>
+          <t>Sorveteria Lafer &amp; Açaí</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -1794,19 +1794,19 @@
       </c>
       <c r="D50" s="2" t="inlineStr">
         <is>
-          <t>6.987</t>
+          <t>982</t>
         </is>
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>R. Artur de Azevedo, 1147</t>
+          <t>R. Maria Curupaiti, 1520</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>OGGI SORVETES PARADA INGLESA</t>
+          <t>Sorveteria do Centro</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -1816,24 +1816,24 @@
       </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D51" s="2" t="inlineStr">
         <is>
-          <t>378</t>
+          <t>2.875</t>
         </is>
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>Av. Gen. Ataliba Leonel, 1976</t>
+          <t>R. Epitácio Pessoa, 94</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>Dezato Gelato - Braz Leme</t>
+          <t>Bacio di Latte Gelato Puro</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -1843,24 +1843,24 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>260</t>
+          <t>1.593</t>
         </is>
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>Av. Braz Leme, 1200 - Loja 06</t>
+          <t>Av. Braz Leme, 2378</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>Sorveteria do Centro</t>
+          <t>Lambisk Sorvetes</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -1870,17 +1870,17 @@
       </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,7</t>
         </is>
       </c>
       <c r="D53" s="2" t="inlineStr">
         <is>
-          <t>2.875</t>
+          <t>192</t>
         </is>
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>R. Epitácio Pessoa, 94</t>
+          <t>R. Conselheiro Moreira de Barros, 1002</t>
         </is>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>Candy Village Sorvete Infancia vintage</t>
+          <t>Bacio di Latte</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -1924,24 +1924,24 @@
       </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D55" s="2" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>808</t>
         </is>
       </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>R. Jovita</t>
+          <t>Tv. Casalbuono, 120</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>Sorveteria Lafer &amp; Açaí</t>
+          <t>Belari Gelato Artesanal - Bairro do Limão</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -1951,24 +1951,24 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>982</t>
+          <t>2.167</t>
         </is>
       </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>R. Maria Curupaiti, 1520</t>
+          <t>Av. Casa Verde, 3527</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>Sou Ice Santa Teresinha - Sorvetes e Congelados</t>
+          <t>Sou ice - Sorvetes e Congelados</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -1978,24 +1978,24 @@
       </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="D57" s="2" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>69</t>
         </is>
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>R. Conselheiro Moreira de Barros, 1309 - Loja 01</t>
+          <t>Av. Nova Cantareira, 346</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>Bacio di Latte Gelato Puro</t>
+          <t>Borelli center norte</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -2005,24 +2005,24 @@
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>1.593</t>
+          <t>96</t>
         </is>
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>Av. Braz Leme, 2378</t>
+          <t>Shopping Center Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>Paraiso dos Sorvetes</t>
+          <t>Italian Dessert</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -2032,24 +2032,24 @@
       </c>
       <c r="C59" s="2" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D59" s="2" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>155</t>
         </is>
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>Av. Conceição, 898</t>
+          <t>R. Dr. Rubens Meireles, 327</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>Sorvete Vintage - Sorvete para eventos | Açaí e Milkshake</t>
+          <t>Frutiquello Sorvetes Vila Guilherme</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -2059,24 +2059,24 @@
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>909</t>
         </is>
       </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>Av. Gen. Ataliba Leonel, 3837</t>
+          <t>Pç. Oscár da Silva, 21</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>Bacio di Latte</t>
+          <t>Candy Village Sorvete Infancia vintage</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -2086,17 +2086,17 @@
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>4,9</t>
         </is>
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>807</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>Tv. Casalbuono, 120</t>
+          <t>R. Jovita</t>
         </is>
       </c>
     </row>

</xml_diff>